<commit_message>
Lectura de información de items (MA y ME)
</commit_message>
<xml_diff>
--- a/src/co/edu/udea/mantpriorivias/archivos/recursos/Alternativas_Intervencion.xlsx
+++ b/src/co/edu/udea/mantpriorivias/archivos/recursos/Alternativas_Intervencion.xlsx
@@ -45,9 +45,6 @@
     <t>TRATAMIENTOS SUPERFICIALES O RIEGOS</t>
   </si>
   <si>
-    <t>Sección transversal inapropiada</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>Drenaje longitudinal inadecuado</t>
-  </si>
-  <si>
     <t>Limpiar las cunetas cada 3 ó 6 meses</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>Construcción e instalación de drenajes longitudinales</t>
   </si>
   <si>
-    <t>Drenaje transversal inadecuado</t>
-  </si>
-  <si>
     <t>Limpiar las alcantarillas y box culverts</t>
   </si>
   <si>
@@ -84,9 +75,6 @@
     <t>Construcción e instalación de drenajes transversales</t>
   </si>
   <si>
-    <t>Ondulaciones</t>
-  </si>
-  <si>
     <t>Perfilar y adicionar material, agua y compactar.</t>
   </si>
   <si>
@@ -108,27 +96,15 @@
     <t>Perfilar y adicionar materiales (agua y agregado, ó 50/50 mezcla de algún estabilizante con grava y compactar)</t>
   </si>
   <si>
-    <t>Surcos y ahuellamiento</t>
-  </si>
-  <si>
     <t>Perfilar y adicionar material, agua y compactar</t>
   </si>
   <si>
-    <t>Cabezas duras</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>Probabilidad  de derrumbes</t>
-  </si>
-  <si>
     <t>Perfilar y vegetalizar los taludes</t>
   </si>
   <si>
-    <t>Daños en la banca</t>
-  </si>
-  <si>
     <t>Nivelación y conformación de la banca</t>
   </si>
   <si>
@@ -192,9 +168,6 @@
     <t>MA8</t>
   </si>
   <si>
-    <t>Bachas</t>
-  </si>
-  <si>
     <t>Cortar la base existente, adicionar agregado, conformar, adicionar agua y compactar.</t>
   </si>
   <si>
@@ -250,6 +223,33 @@
   </si>
   <si>
     <t>Agregado Suelto</t>
+  </si>
+  <si>
+    <t>Baches / Huecos</t>
+  </si>
+  <si>
+    <t>Ahuellamiento / Surcos</t>
+  </si>
+  <si>
+    <t>Cabezas Duras</t>
+  </si>
+  <si>
+    <t>Probabilidad  de Derrumbes</t>
+  </si>
+  <si>
+    <t>Daños en la Banca</t>
+  </si>
+  <si>
+    <t>Sección Transversal Inapropiada</t>
+  </si>
+  <si>
+    <t>Drenaje Longitudinal Inadecuado</t>
+  </si>
+  <si>
+    <t>Drenaje Transversal Inadecuado</t>
+  </si>
+  <si>
+    <t>Corrugaciones</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -425,24 +425,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,6 +489,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,7 +878,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,526 +894,526 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="C36" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-    </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-    </row>
-    <row r="28" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-    </row>
-    <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-    </row>
-    <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1411,7 +1428,7 @@
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A29:A33"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="A34:A36"/>

</xml_diff>

<commit_message>
Actualización documentación Alternativas Intervención
</commit_message>
<xml_diff>
--- a/src/co/edu/udea/mantpriorivias/archivos/recursos/Alternativas_Intervencion.xlsx
+++ b/src/co/edu/udea/mantpriorivias/archivos/recursos/Alternativas_Intervencion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andersson\Desktop\Temporales\mantenimiento-priorizacion-vias\src\co\edu\udea\mantpriorivias\archivos\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andersson\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="ALTERNATIVAS DE INTERVENCIÓN" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>MANTENIMIENTO</t>
   </si>
@@ -51,69 +51,24 @@
     <t>M</t>
   </si>
   <si>
-    <t>Perfilar y adicionar material, agua y compactar.</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
     <t>Limpiar las cunetas cada 3 ó 6 meses</t>
   </si>
   <si>
-    <t>Reconformar y ampliar las cunetas</t>
-  </si>
-  <si>
-    <t>Construcción e instalación de drenajes longitudinales</t>
-  </si>
-  <si>
-    <t>Limpiar las alcantarillas y box culverts</t>
-  </si>
-  <si>
     <t>Construcción de nuevas alcantarillas y mejoramiento de las ya existentes</t>
   </si>
   <si>
-    <t>Construcción e instalación de drenajes transversales</t>
-  </si>
-  <si>
-    <t>Perfilar y adicionar material, agua y compactar.</t>
-  </si>
-  <si>
-    <t>Cortar la base, adicionar agregado, conformar, adicionar agua y compactar.</t>
-  </si>
-  <si>
-    <t>Polvo</t>
-  </si>
-  <si>
-    <t>Adicionar agua</t>
-  </si>
-  <si>
-    <t>Adicionar algún estabilizante control polvo</t>
-  </si>
-  <si>
     <t>Reaplicación localizada de grava</t>
   </si>
   <si>
-    <t>Perfilar y adicionar materiales (agua y agregado, ó 50/50 mezcla de algún estabilizante con grava y compactar)</t>
-  </si>
-  <si>
-    <t>Perfilar y adicionar material, agua y compactar</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>Perfilar y vegetalizar los taludes</t>
-  </si>
-  <si>
     <t>Nivelación y conformación de la banca</t>
   </si>
   <si>
-    <t>Construir llenos para estabilizar la banca</t>
-  </si>
-  <si>
-    <t>Construir obras de contención</t>
-  </si>
-  <si>
     <t>MA1</t>
   </si>
   <si>
@@ -159,51 +114,21 @@
     <t>MA21</t>
   </si>
   <si>
-    <t>MA22</t>
-  </si>
-  <si>
     <t>MA2</t>
   </si>
   <si>
     <t>MA8</t>
   </si>
   <si>
-    <t>cortar la base existente,adicionar un estabilizante control polvo, agua y compactar</t>
-  </si>
-  <si>
-    <t>Cortar la base existente ,adicionar agregado, estabilizante, conformar, adicionar agua y compactar.</t>
-  </si>
-  <si>
-    <t>Cortar la base existente, adicionar agregado, conformar, adicionar agua y compactar</t>
-  </si>
-  <si>
-    <t>Perfilar el terreno (no incluye adición de material)conformar y compactar</t>
-  </si>
-  <si>
     <t>MA5</t>
   </si>
   <si>
-    <t>Perfilado ligero (no contempla adición de materiales) conformar y compactar</t>
-  </si>
-  <si>
-    <t>Perfilado ligero (no contempla adición de materiales) conformar y compactar.</t>
-  </si>
-  <si>
-    <t>Construir obras de disipación de energía</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Construir sistemas de drenaje para taludes </t>
-  </si>
-  <si>
     <t>MA16</t>
   </si>
   <si>
     <t xml:space="preserve">Construir obras de estabilización de taludes </t>
   </si>
   <si>
-    <t>Construir obras de contención para taludes</t>
-  </si>
-  <si>
     <t>MA18</t>
   </si>
   <si>
@@ -213,40 +138,91 @@
     <t>° Slurry Seal (ME1)                                                                  ° Mapia (ME2)                                                                          ° Micropavimento (ME3)                                                 ° Tratamiento superficial simple (ME5)                      ° Tratamiento superficial doble (ME4)</t>
   </si>
   <si>
-    <t>Agregado Suelto</t>
-  </si>
-  <si>
-    <t>Baches / Huecos</t>
-  </si>
-  <si>
-    <t>Ahuellamiento / Surcos</t>
-  </si>
-  <si>
-    <t>Cabezas Duras</t>
-  </si>
-  <si>
-    <t>Probabilidad  de Derrumbes</t>
-  </si>
-  <si>
-    <t>Daños en la Banca</t>
-  </si>
-  <si>
-    <t>Sección Transversal Inapropiada</t>
-  </si>
-  <si>
-    <t>Drenaje Longitudinal Inadecuado</t>
-  </si>
-  <si>
-    <t>Drenaje Transversal Inadecuado</t>
-  </si>
-  <si>
-    <t>Corrugaciones</t>
-  </si>
-  <si>
     <t>° Estabilización Física (ME6)                                                      ° Estabilización Química (ME7)                                                ° Estabilización Mecánica (ME8)</t>
   </si>
   <si>
-    <t>Perfilado ligero (no contempla adición de materiales) conformar  y compactar</t>
+    <t>Perfilado ligero (no contempla adición de materiales), incluye conformación  y compactación</t>
+  </si>
+  <si>
+    <t>Perfilado y adición de material y agua; incluye conformación y compactación</t>
+  </si>
+  <si>
+    <t>Corte de la base existente, adición de agregado, y agua; incluye conformación y compactación</t>
+  </si>
+  <si>
+    <t>conformación  y ampliación de las cunetas</t>
+  </si>
+  <si>
+    <t>Construcción e instalación de sistemas de drenaje longitudinales</t>
+  </si>
+  <si>
+    <t>Limpieza de las alcantarillas y box culverts</t>
+  </si>
+  <si>
+    <t>Construcción e instalación de sistemas de drenajes transversales</t>
+  </si>
+  <si>
+    <t>Adición de agua</t>
+  </si>
+  <si>
+    <t>Adición de algún estabilizante control polvo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corte de la base existente,adición de un estabilizante control polvo y agua; incluye conformación y compactación </t>
+  </si>
+  <si>
+    <t>Perfilado  y vegetalización de los taludes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construcción de sistemas de drenaje para taludes </t>
+  </si>
+  <si>
+    <t>Construcción de  obras de disipación de energía</t>
+  </si>
+  <si>
+    <t>Construcción de obras de contención para taludes</t>
+  </si>
+  <si>
+    <t>Construcción de llenos para estabilización de  la banca</t>
+  </si>
+  <si>
+    <t>Construcción de obras de contención para estabilización de la banca</t>
+  </si>
+  <si>
+    <t>Sección Transversal Inapropiada (81)</t>
+  </si>
+  <si>
+    <t>Drenaje Longitudinal Inadecuado (82)</t>
+  </si>
+  <si>
+    <t>Drenaje Transversal Inadecuado (83)</t>
+  </si>
+  <si>
+    <t>Corrugaciones (84)</t>
+  </si>
+  <si>
+    <t>Polvo (85)</t>
+  </si>
+  <si>
+    <t>Baches / Huecos (86)</t>
+  </si>
+  <si>
+    <t>Ahuellamiento / Surcos (87)</t>
+  </si>
+  <si>
+    <t>Agregado Suelto (88)</t>
+  </si>
+  <si>
+    <t>Cabezas Duras (89)</t>
+  </si>
+  <si>
+    <t>Probabilidad  de Derrumbes (90)</t>
+  </si>
+  <si>
+    <t>Daños en la Banca (91)</t>
+  </si>
+  <si>
+    <t>CÓDIGO DE MANTENIMIENTO</t>
   </si>
 </sst>
 </file>
@@ -437,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -452,6 +428,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -880,7 +859,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="12.5703125"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -891,24 +870,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -920,7 +899,9 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
@@ -928,489 +909,489 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>69</v>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>62</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>70</v>
+      <c r="A7" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>71</v>
+      <c r="A10" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>72</v>
+        <v>20</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>19</v>
+      <c r="A16" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>64</v>
+      <c r="A19" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>65</v>
+        <v>22</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>63</v>
+        <v>22</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="54.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>67</v>
+      <c r="A29" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="12" t="s">
-        <v>10</v>
+      <c r="A32" s="11"/>
+      <c r="B32" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="13"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>68</v>
+      <c r="A34" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
       <c r="B35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
       <c r="B36" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>